<commit_message>
Updated files and refactored demographics.py
</commit_message>
<xml_diff>
--- a/tests/demo/demo_lob.xlsx
+++ b/tests/demo/demo_lob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optum\hm-automation\tests\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBD3EC3-7A20-4172-8F7C-3CAAEB3CC4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9162FC21-1CD3-47FE-9E74-98D9B58F44F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>First Name</t>
   </si>
@@ -49,12 +49,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>plan_card_1</t>
-  </si>
-  <si>
-    <t>Test ID</t>
-  </si>
-  <si>
     <t>App Type</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>Parent Question</t>
   </si>
   <si>
-    <t>Plans</t>
-  </si>
-  <si>
     <t>xxx</t>
   </si>
   <si>
@@ -94,9 +85,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>plan_card_2</t>
-  </si>
-  <si>
     <t>asd</t>
   </si>
   <si>
@@ -116,9 +104,6 @@
   </si>
   <si>
     <t>Vision Insurance</t>
-  </si>
-  <si>
-    <t>plan_card_3</t>
   </si>
   <si>
     <t>Supplemental Insurance</t>
@@ -510,322 +495,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4">
+        <v>30008</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4">
-        <v>30008</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9999999999</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="4">
+        <v>30007</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45002</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4">
+        <v>17001</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4">
+        <v>30009</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4">
-        <v>30007</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4">
+        <v>45001</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1">
         <v>9999999999</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>21</v>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4">
-        <v>45002</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9999999999</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4">
-        <v>17001</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9999999999</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="4">
-        <v>30009</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1">
-        <v>9999999999</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4">
-        <v>45001</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9999999999</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D8"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{9988CF25-EECD-4A7B-AC04-2CCA166C5011}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{9988CF25-EECD-4A7B-AC04-2CCA166C5011}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>